<commit_message>
Added handling of common packages.
</commit_message>
<xml_diff>
--- a/data/backend/activity-service_structure.xlsx
+++ b/data/backend/activity-service_structure.xlsx
@@ -1437,93 +1437,93 @@
     <t>NULL_PAGE_ERROR_MESSAGE</t>
   </si>
   <si>
+    <t>operationHttpStatusMapper</t>
+  </si>
+  <si>
+    <t>org.andante.mappers.OperationHttpStatusMapper</t>
+  </si>
+  <si>
+    <t>IDENTIFIERS_LIST_NULL_MESSAGE</t>
+  </si>
+  <si>
+    <t>NEGATIVE_PAGE_ERROR_MESSAGE</t>
+  </si>
+  <si>
+    <t>ACTIVITY_EMAIL_NOT_VALID_MESSAGE</t>
+  </si>
+  <si>
+    <t>activityService</t>
+  </si>
+  <si>
+    <t>activityDTOModelMapper</t>
+  </si>
+  <si>
+    <t>NULL_PAGE_SIZE_ERROR_MESSAGE</t>
+  </si>
+  <si>
     <t>NON_POSITIVE_PAGE_SIZE_MESSAGE</t>
   </si>
   <si>
-    <t>operationHttpStatusMapper</t>
-  </si>
-  <si>
-    <t>org.andante.mappers.OperationHttpStatusMapper</t>
-  </si>
-  <si>
-    <t>NULL_PAGE_SIZE_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>IDENTIFIERS_LIST_NULL_MESSAGE</t>
-  </si>
-  <si>
-    <t>activityService</t>
+    <t>ACTIVITY_IDENTIFIER_NOT_BLANK_MESSAGE</t>
   </si>
   <si>
     <t>IDENTIFIERS_LIST_MESSAGE</t>
   </si>
   <si>
-    <t>ACTIVITY_EMAIL_NOT_VALID_MESSAGE</t>
-  </si>
-  <si>
-    <t>activityDTOModelMapper</t>
-  </si>
-  <si>
     <t>ACTIVITY_EMAIL_BLANK_MESSAGE</t>
   </si>
   <si>
-    <t>NEGATIVE_PAGE_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>ACTIVITY_IDENTIFIER_NOT_BLANK_MESSAGE</t>
-  </si>
-  <si>
     <t>$SwitchMap$org$andante$enums$OperationType</t>
   </si>
   <si>
     <t>int[]</t>
   </si>
   <si>
+    <t>affectedUsers</t>
+  </si>
+  <si>
+    <t>acknowledgedUsers</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>relatedId</t>
+  </si>
+  <si>
+    <t>eventTimestamp</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
     <t>affectsAll</t>
   </si>
   <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>affectedUsers</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>eventTimestamp</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>acknowledgedUsers</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>relatedId</t>
-  </si>
-  <si>
     <t>decoder</t>
   </si>
   <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>observedUsers</t>
+  </si>
+  <si>
+    <t>communityImageUrl</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
     <t>imageUrl</t>
   </si>
   <si>
-    <t>communityImageUrl</t>
-  </si>
-  <si>
-    <t>observedUsers</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
     <t>observingUsers</t>
   </si>
   <si>
@@ -1536,45 +1536,45 @@
     <t>java.lang.Integer</t>
   </si>
   <si>
+    <t>enableStartTLS</t>
+  </si>
+  <si>
+    <t>smtpAuth</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>host</t>
   </si>
   <si>
-    <t>enableStartTLS</t>
-  </si>
-  <si>
-    <t>smtpAuth</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>USERNAME_NULL_ERROR_MESSAGE</t>
+  </si>
+  <si>
+    <t>IDENTIFIERS_LIST_NULL_ERROR_MESSAGE</t>
+  </si>
+  <si>
+    <t>jwtTokenDecoder</t>
   </si>
   <si>
     <t>profileService</t>
   </si>
   <si>
+    <t>userProfileService</t>
+  </si>
+  <si>
+    <t>USERNAME_BLANK_ERROR_MESSAGE</t>
+  </si>
+  <si>
     <t>IDENTIFIERS_LIST_SIZE_ERROR_MESSAGE</t>
   </si>
   <si>
-    <t>jwtTokenDecoder</t>
-  </si>
-  <si>
-    <t>IDENTIFIERS_LIST_NULL_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>USERNAME_NULL_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>USERNAME_BLANK_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>userProfileService</t>
+    <t>userProfileMapper</t>
   </si>
   <si>
     <t>IMAGE_URL_BLANK_ERROR_MESSAGE</t>
   </si>
   <si>
-    <t>userProfileMapper</t>
-  </si>
-  <si>
     <t>affectsAll$value</t>
   </si>
   <si>
@@ -1593,39 +1593,42 @@
     <t>keycloakUpdateUserPath</t>
   </si>
   <si>
+    <t>keycloakGetUserPath</t>
+  </si>
+  <si>
+    <t>keycloakUrl</t>
+  </si>
+  <si>
+    <t>keycloakAdminTokenPath</t>
+  </si>
+  <si>
+    <t>adminUsername</t>
+  </si>
+  <si>
     <t>adminPassword</t>
   </si>
   <si>
-    <t>adminUsername</t>
-  </si>
-  <si>
-    <t>keycloakUrl</t>
-  </si>
-  <si>
-    <t>keycloakGetUserPath</t>
-  </si>
-  <si>
-    <t>keycloakAdminTokenPath</t>
-  </si>
-  <si>
     <t>observed</t>
   </si>
   <si>
     <t>observers</t>
   </si>
   <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>org.springframework.core.io.Resource</t>
+  </si>
+  <si>
+    <t>NEWSLETTER_TEMPLATE</t>
+  </si>
+  <si>
+    <t>NEWSLETTER_TITLE</t>
+  </si>
+  <si>
     <t>sender</t>
   </si>
   <si>
-    <t>logo</t>
-  </si>
-  <si>
-    <t>org.springframework.core.io.Resource</t>
-  </si>
-  <si>
-    <t>NEWSLETTER_TITLE</t>
-  </si>
-  <si>
     <t>mailSender</t>
   </si>
   <si>
@@ -1635,7 +1638,10 @@
     <t>org.thymeleaf.TemplateEngine</t>
   </si>
   <si>
-    <t>NEWSLETTER_TEMPLATE</t>
+    <t>USER_NOT_FOUND_EXCEPTION_MESSAGE</t>
+  </si>
+  <si>
+    <t>userProfileRepository</t>
   </si>
   <si>
     <t>USER_CONFLICT_EXCEPTION_MESSAGE</t>
@@ -1644,127 +1650,121 @@
     <t>userProfileModelEntityMapper</t>
   </si>
   <si>
-    <t>USER_NOT_FOUND_EXCEPTION_MESSAGE</t>
-  </si>
-  <si>
-    <t>userProfileRepository</t>
-  </si>
-  <si>
     <t>issuerUri</t>
   </si>
   <si>
+    <t>NEWSLETTER_NOT_FOUND_EXCEPTION_MESSAGE</t>
+  </si>
+  <si>
+    <t>newsletterRepository</t>
+  </si>
+  <si>
     <t>newsletterMapper</t>
   </si>
   <si>
     <t>NEWSLETTER_CONFLICT_EXCEPTION_MESSAGE</t>
   </si>
   <si>
-    <t>NEWSLETTER_NOT_FOUND_EXCEPTION_MESSAGE</t>
-  </si>
-  <si>
-    <t>newsletterRepository</t>
+    <t>privateToken</t>
   </si>
   <si>
     <t>databaseId</t>
   </si>
   <si>
-    <t>privateToken</t>
-  </si>
-  <si>
     <t>bootstrapServers</t>
   </si>
   <si>
+    <t>USER_NOT_AFFECTED_EXCEPTION_MESSAGE</t>
+  </si>
+  <si>
+    <t>activityModelEntityMapper</t>
+  </si>
+  <si>
+    <t>ACTIVITY_CONFLICT_EXCEPTION_MESSAGE</t>
+  </si>
+  <si>
     <t>ACTIVITY_NOT_FOUND_EXCEPTION_MESSAGE</t>
   </si>
   <si>
-    <t>USER_NOT_AFFECTED_EXCEPTION_MESSAGE</t>
-  </si>
-  <si>
     <t>rsqlParser</t>
   </si>
   <si>
     <t>cz.jirutka.rsql.parser.RSQLParser</t>
   </si>
   <si>
-    <t>ACTIVITY_CONFLICT_EXCEPTION_MESSAGE</t>
-  </si>
-  <si>
-    <t>activityModelEntityMapper</t>
+    <t>rsqlVisitor</t>
+  </si>
+  <si>
+    <t>org.andante.rsql.PersistentRSQLVisitor</t>
   </si>
   <si>
     <t>activityRepository</t>
   </si>
   <si>
-    <t>rsqlVisitor</t>
-  </si>
-  <si>
-    <t>org.andante.rsql.PersistentRSQLVisitor</t>
+    <t>emailSender</t>
+  </si>
+  <si>
+    <t>newsletterService</t>
+  </si>
+  <si>
+    <t>EMAIL_BLANK_ERROR_MESSAGE</t>
   </si>
   <si>
     <t>EMAIL_NOT_VALID_ERROR_MESSAGE</t>
   </si>
   <si>
-    <t>emailSender</t>
-  </si>
-  <si>
-    <t>EMAIL_BLANK_ERROR_MESSAGE</t>
-  </si>
-  <si>
-    <t>newsletterService</t>
-  </si>
-  <si>
     <t>activityConfiguration</t>
   </si>
   <si>
+    <t>entrySet</t>
+  </si>
+  <si>
+    <t>DEFAULT_LOAD_FACTOR</t>
+  </si>
+  <si>
+    <t>this$0</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>keySet</t>
+  </si>
+  <si>
+    <t>UNTREEIFY_THRESHOLD</t>
+  </si>
+  <si>
+    <t>DEFAULT_INITIAL_CAPACITY</t>
+  </si>
+  <si>
+    <t>MAXIMUM_CAPACITY</t>
+  </si>
+  <si>
     <t>val$productOutputDTO</t>
   </si>
   <si>
     <t>org.andante.product.dto.ProductOutputDTO</t>
   </si>
   <si>
+    <t>loadFactor</t>
+  </si>
+  <si>
+    <t>modCount</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
     <t>TREEIFY_THRESHOLD</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>threshold</t>
-  </si>
-  <si>
-    <t>UNTREEIFY_THRESHOLD</t>
-  </si>
-  <si>
     <t>MIN_TREEIFY_CAPACITY</t>
   </si>
   <si>
-    <t>loadFactor</t>
-  </si>
-  <si>
     <t>table</t>
   </si>
   <si>
     <t>values</t>
-  </si>
-  <si>
-    <t>DEFAULT_INITIAL_CAPACITY</t>
-  </si>
-  <si>
-    <t>modCount</t>
-  </si>
-  <si>
-    <t>DEFAULT_LOAD_FACTOR</t>
-  </si>
-  <si>
-    <t>MAXIMUM_CAPACITY</t>
-  </si>
-  <si>
-    <t>this$0</t>
-  </si>
-  <si>
-    <t>keySet</t>
-  </si>
-  <si>
-    <t>entrySet</t>
   </si>
   <si>
     <t>Source Class Name</t>
@@ -24034,7 +24034,7 @@
         <v>47</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>14</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4">
@@ -24042,13 +24042,13 @@
         <v>456</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>473</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -24104,7 +24104,7 @@
         <v>47</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
@@ -24132,7 +24132,7 @@
         <v>47</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -24244,7 +24244,7 @@
         <v>47</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>86</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
@@ -24258,7 +24258,7 @@
         <v>47</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -24272,7 +24272,7 @@
         <v>47</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -24286,7 +24286,7 @@
         <v>47</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
@@ -24300,7 +24300,7 @@
         <v>47</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -24314,7 +24314,7 @@
         <v>47</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24">
@@ -24328,7 +24328,7 @@
         <v>47</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -24342,7 +24342,7 @@
         <v>47</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
@@ -24356,7 +24356,7 @@
         <v>47</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>14</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27">
@@ -24440,7 +24440,7 @@
         <v>47</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
@@ -24468,7 +24468,7 @@
         <v>47</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -24602,7 +24602,7 @@
         <v>145</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>47</v>
@@ -24616,7 +24616,7 @@
         <v>145</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>47</v>
@@ -24630,7 +24630,7 @@
         <v>145</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>47</v>
@@ -24644,7 +24644,7 @@
         <v>145</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="C47" t="s" s="0">
         <v>47</v>
@@ -24678,7 +24678,7 @@
         <v>47</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>95</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -24720,7 +24720,7 @@
         <v>47</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>14</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53">
@@ -24734,7 +24734,7 @@
         <v>47</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -24762,7 +24762,7 @@
         <v>47</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
@@ -24776,7 +24776,7 @@
         <v>47</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57">
@@ -24790,7 +24790,7 @@
         <v>47</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>125</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58">
@@ -24812,13 +24812,13 @@
         <v>12</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C59" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60">
@@ -24826,7 +24826,7 @@
         <v>12</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C60" t="s" s="0">
         <v>47</v>
@@ -24840,7 +24840,7 @@
         <v>12</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C61" t="s" s="0">
         <v>47</v>
@@ -24854,7 +24854,7 @@
         <v>12</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C62" t="s" s="0">
         <v>47</v>
@@ -24882,13 +24882,13 @@
         <v>12</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C64" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65">
@@ -24910,13 +24910,13 @@
         <v>183</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67">
@@ -24924,13 +24924,13 @@
         <v>183</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>517</v>
+        <v>485</v>
       </c>
       <c r="C67" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>86</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68">
@@ -24938,13 +24938,13 @@
         <v>183</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>487</v>
+        <v>517</v>
       </c>
       <c r="C68" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69">
@@ -24952,13 +24952,13 @@
         <v>183</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>518</v>
+        <v>490</v>
       </c>
       <c r="C69" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>7</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70">
@@ -24966,13 +24966,13 @@
         <v>183</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="C70" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
@@ -24980,7 +24980,7 @@
         <v>183</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>47</v>
@@ -24994,13 +24994,13 @@
         <v>183</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="C72" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73">
@@ -25014,7 +25014,7 @@
         <v>47</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74">
@@ -25022,7 +25022,7 @@
         <v>183</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C74" t="s" s="0">
         <v>47</v>
@@ -25036,13 +25036,13 @@
         <v>183</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C75" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76">
@@ -25148,13 +25148,13 @@
         <v>208</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="C83" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D83" t="s" s="0">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
@@ -25162,7 +25162,7 @@
         <v>208</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C84" t="s" s="0">
         <v>47</v>
@@ -25176,7 +25176,7 @@
         <v>208</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C85" t="s" s="0">
         <v>47</v>
@@ -25190,7 +25190,7 @@
         <v>208</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C86" t="s" s="0">
         <v>47</v>
@@ -25204,13 +25204,13 @@
         <v>208</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>514</v>
+        <v>527</v>
       </c>
       <c r="C87" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88">
@@ -25218,13 +25218,13 @@
         <v>224</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D88" t="s" s="0">
-        <v>86</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89">
@@ -25232,13 +25232,13 @@
         <v>224</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90">
@@ -25246,13 +25246,13 @@
         <v>224</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91">
@@ -25260,13 +25260,13 @@
         <v>201</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D91" t="s" s="0">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92">
@@ -25288,13 +25288,13 @@
         <v>201</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94">
@@ -25316,13 +25316,13 @@
         <v>235</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c r="C95" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96">
@@ -25344,7 +25344,7 @@
         <v>235</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>488</v>
+        <v>499</v>
       </c>
       <c r="C97" t="s" s="0">
         <v>47</v>
@@ -25358,13 +25358,13 @@
         <v>235</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>495</v>
+        <v>529</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99">
@@ -25372,13 +25372,13 @@
         <v>235</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>528</v>
+        <v>498</v>
       </c>
       <c r="C99" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -25386,13 +25386,13 @@
         <v>235</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>529</v>
+        <v>491</v>
       </c>
       <c r="C100" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -25434,7 +25434,7 @@
         <v>47</v>
       </c>
       <c r="D103" t="s" s="0">
-        <v>14</v>
+        <v>531</v>
       </c>
     </row>
     <row r="104">
@@ -25442,13 +25442,13 @@
         <v>251</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C104" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D104" t="s" s="0">
-        <v>532</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -25476,7 +25476,7 @@
         <v>47</v>
       </c>
       <c r="D106" t="s" s="0">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107">
@@ -25490,7 +25490,7 @@
         <v>47</v>
       </c>
       <c r="D107" t="s" s="0">
-        <v>536</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108">
@@ -25498,13 +25498,13 @@
         <v>251</v>
       </c>
       <c r="B108" t="s" s="0">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C108" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D108" t="s" s="0">
-        <v>14</v>
+        <v>537</v>
       </c>
     </row>
     <row r="109">
@@ -25546,7 +25546,7 @@
         <v>47</v>
       </c>
       <c r="D111" t="s" s="0">
-        <v>285</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112">
@@ -25574,7 +25574,7 @@
         <v>47</v>
       </c>
       <c r="D113" t="s" s="0">
-        <v>115</v>
+        <v>285</v>
       </c>
     </row>
     <row r="114">
@@ -25602,7 +25602,7 @@
         <v>47</v>
       </c>
       <c r="D115" t="s" s="0">
-        <v>172</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116">
@@ -25616,7 +25616,7 @@
         <v>47</v>
       </c>
       <c r="D116" t="s" s="0">
-        <v>14</v>
+        <v>89</v>
       </c>
     </row>
     <row r="117">
@@ -25630,7 +25630,7 @@
         <v>47</v>
       </c>
       <c r="D117" t="s" s="0">
-        <v>14</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118">
@@ -25644,7 +25644,7 @@
         <v>47</v>
       </c>
       <c r="D118" t="s" s="0">
-        <v>89</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -25652,13 +25652,13 @@
         <v>236</v>
       </c>
       <c r="B119" t="s" s="0">
-        <v>528</v>
+        <v>491</v>
       </c>
       <c r="C119" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D119" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120">
@@ -25666,13 +25666,13 @@
         <v>236</v>
       </c>
       <c r="B120" t="s" s="0">
-        <v>529</v>
+        <v>499</v>
       </c>
       <c r="C120" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D120" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121">
@@ -25680,13 +25680,13 @@
         <v>236</v>
       </c>
       <c r="B121" t="s" s="0">
-        <v>496</v>
+        <v>529</v>
       </c>
       <c r="C121" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D121" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="122">
@@ -25694,7 +25694,7 @@
         <v>236</v>
       </c>
       <c r="B122" t="s" s="0">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="C122" t="s" s="0">
         <v>47</v>
@@ -25708,13 +25708,13 @@
         <v>236</v>
       </c>
       <c r="B123" t="s" s="0">
-        <v>495</v>
+        <v>528</v>
       </c>
       <c r="C123" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D123" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="124">
@@ -25764,7 +25764,7 @@
         <v>285</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C127" t="s" s="0">
         <v>47</v>
@@ -25854,7 +25854,7 @@
         <v>47</v>
       </c>
       <c r="D133" t="s" s="0">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="134">
@@ -25868,7 +25868,7 @@
         <v>47</v>
       </c>
       <c r="D134" t="s" s="0">
-        <v>553</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135">
@@ -25876,7 +25876,7 @@
         <v>329</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C135" t="s" s="0">
         <v>47</v>
@@ -25890,13 +25890,13 @@
         <v>329</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C136" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>53</v>
+        <v>555</v>
       </c>
     </row>
     <row r="137">
@@ -25910,7 +25910,7 @@
         <v>47</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>357</v>
+        <v>557</v>
       </c>
     </row>
     <row r="138">
@@ -25918,13 +25918,13 @@
         <v>329</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C138" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>558</v>
+        <v>357</v>
       </c>
     </row>
     <row r="139">
@@ -25946,13 +25946,13 @@
         <v>74</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C140" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D140" t="s" s="0">
-        <v>86</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141">
@@ -25960,13 +25960,13 @@
         <v>74</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C141" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D141" t="s" s="0">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="142">
@@ -25974,13 +25974,13 @@
         <v>74</v>
       </c>
       <c r="B142" t="s" s="0">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C142" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D142" t="s" s="0">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="143">
@@ -25994,7 +25994,7 @@
         <v>47</v>
       </c>
       <c r="D143" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144">
@@ -26002,13 +26002,13 @@
         <v>74</v>
       </c>
       <c r="B144" t="s" s="0">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="C144" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D144" t="s" s="0">
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145">
@@ -26016,13 +26016,13 @@
         <v>74</v>
       </c>
       <c r="B145" t="s" s="0">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C145" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D145" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="146">
@@ -26030,13 +26030,13 @@
         <v>74</v>
       </c>
       <c r="B146" t="s" s="0">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C146" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D146" t="s" s="0">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="147">
@@ -26044,13 +26044,13 @@
         <v>74</v>
       </c>
       <c r="B147" t="s" s="0">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C147" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D147" t="s" s="0">
-        <v>83</v>
+        <v>18</v>
       </c>
     </row>
     <row r="148">
@@ -26058,13 +26058,13 @@
         <v>74</v>
       </c>
       <c r="B148" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C148" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D148" t="s" s="0">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="149">
@@ -26092,7 +26092,7 @@
         <v>47</v>
       </c>
       <c r="D150" t="s" s="0">
-        <v>14</v>
+        <v>251</v>
       </c>
     </row>
     <row r="151">
@@ -26106,7 +26106,7 @@
         <v>47</v>
       </c>
       <c r="D151" t="s" s="0">
-        <v>251</v>
+        <v>220</v>
       </c>
     </row>
     <row r="152">
@@ -26128,7 +26128,7 @@
         <v>465</v>
       </c>
       <c r="B153" t="s" s="0">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C153" t="s" s="0">
         <v>47</v>
@@ -26148,7 +26148,7 @@
         <v>47</v>
       </c>
       <c r="D154" t="s" s="0">
-        <v>220</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155">
@@ -26198,13 +26198,13 @@
         <v>174</v>
       </c>
       <c r="B158" t="s" s="0">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C158" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D158" t="s" s="0">
-        <v>86</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159">
@@ -26212,13 +26212,13 @@
         <v>174</v>
       </c>
       <c r="B159" t="s" s="0">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C159" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D159" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160">
@@ -26226,13 +26226,13 @@
         <v>174</v>
       </c>
       <c r="B160" t="s" s="0">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C160" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D160" t="s" s="0">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="161">
@@ -26282,13 +26282,13 @@
         <v>43</v>
       </c>
       <c r="B164" t="s" s="0">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="C164" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D164" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="165">
@@ -26296,13 +26296,13 @@
         <v>43</v>
       </c>
       <c r="B165" t="s" s="0">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="C165" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D165" t="s" s="0">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="166">
@@ -26310,13 +26310,13 @@
         <v>43</v>
       </c>
       <c r="B166" t="s" s="0">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C166" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D166" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="167">
@@ -26324,13 +26324,13 @@
         <v>43</v>
       </c>
       <c r="B167" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C167" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D167" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168">
@@ -26338,7 +26338,7 @@
         <v>43</v>
       </c>
       <c r="B168" t="s" s="0">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="C168" t="s" s="0">
         <v>47</v>
@@ -26352,7 +26352,7 @@
         <v>43</v>
       </c>
       <c r="B169" t="s" s="0">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C169" t="s" s="0">
         <v>47</v>
@@ -26366,13 +26366,13 @@
         <v>43</v>
       </c>
       <c r="B170" t="s" s="0">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C170" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D170" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171">
@@ -26380,13 +26380,13 @@
         <v>43</v>
       </c>
       <c r="B171" t="s" s="0">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C171" t="s" s="0">
         <v>47</v>
       </c>
       <c r="D171" t="s" s="0">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="172">
@@ -26394,7 +26394,7 @@
         <v>43</v>
       </c>
       <c r="B172" t="s" s="0">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C172" t="s" s="0">
         <v>47</v>
@@ -26414,7 +26414,7 @@
         <v>111</v>
       </c>
       <c r="D173" t="s" s="0">
-        <v>565</v>
+        <v>18</v>
       </c>
     </row>
     <row r="174">
@@ -26422,13 +26422,13 @@
         <v>380</v>
       </c>
       <c r="B174" t="s" s="0">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C174" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D174" t="s" s="0">
-        <v>23</v>
+        <v>440</v>
       </c>
     </row>
     <row r="175">
@@ -26436,13 +26436,13 @@
         <v>380</v>
       </c>
       <c r="B175" t="s" s="0">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C175" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D175" t="s" s="0">
-        <v>23</v>
+        <v>373</v>
       </c>
     </row>
     <row r="176">
@@ -26450,7 +26450,7 @@
         <v>380</v>
       </c>
       <c r="B176" t="s" s="0">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C176" t="s" s="0">
         <v>111</v>
@@ -26464,13 +26464,13 @@
         <v>380</v>
       </c>
       <c r="B177" t="s" s="0">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C177" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D177" t="s" s="0">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="178">
@@ -26478,7 +26478,7 @@
         <v>380</v>
       </c>
       <c r="B178" t="s" s="0">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C178" t="s" s="0">
         <v>111</v>
@@ -26492,13 +26492,13 @@
         <v>380</v>
       </c>
       <c r="B179" t="s" s="0">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C179" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D179" t="s" s="0">
-        <v>440</v>
+        <v>23</v>
       </c>
     </row>
     <row r="180">
@@ -26506,13 +26506,13 @@
         <v>380</v>
       </c>
       <c r="B180" t="s" s="0">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C180" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D180" t="s" s="0">
-        <v>443</v>
+        <v>23</v>
       </c>
     </row>
     <row r="181">
@@ -26520,13 +26520,13 @@
         <v>380</v>
       </c>
       <c r="B181" t="s" s="0">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C181" t="s" s="0">
         <v>111</v>
       </c>
       <c r="D181" t="s" s="0">
-        <v>430</v>
+        <v>573</v>
       </c>
     </row>
     <row r="182">
@@ -26540,7 +26540,7 @@
         <v>111</v>
       </c>
       <c r="D182" t="s" s="0">
-        <v>23</v>
+        <v>440</v>
       </c>
     </row>
     <row r="183">
@@ -26568,7 +26568,7 @@
         <v>111</v>
       </c>
       <c r="D184" t="s" s="0">
-        <v>440</v>
+        <v>23</v>
       </c>
     </row>
     <row r="185">
@@ -26596,7 +26596,7 @@
         <v>111</v>
       </c>
       <c r="D186" t="s" s="0">
-        <v>373</v>
+        <v>23</v>
       </c>
     </row>
     <row r="187">
@@ -26610,7 +26610,7 @@
         <v>111</v>
       </c>
       <c r="D187" t="s" s="0">
-        <v>18</v>
+        <v>443</v>
       </c>
     </row>
     <row r="188">
@@ -26624,7 +26624,7 @@
         <v>111</v>
       </c>
       <c r="D188" t="s" s="0">
-        <v>18</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>